<commit_message>
kinda add server configuration form but it doesn't work
</commit_message>
<xml_diff>
--- a/Plugins.xlsx
+++ b/Plugins.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Skiuileuf\Documents\UiPath\ActualizarePluginuriServerMinecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB244939-458C-4C65-ACB7-F7239F4A9039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6A1C6C-7F5A-4C2A-BB08-BD9492CE6C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMP" sheetId="1" r:id="rId1"/>
     <sheet name="Lobby" sheetId="2" r:id="rId2"/>
+    <sheet name="Velocity" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="51">
   <si>
     <t>Nume</t>
   </si>
@@ -185,10 +186,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,13 +220,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +551,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
@@ -575,7 +587,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
@@ -749,6 +761,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{B9B917E1-554F-4C21-8DEF-DD1DEB24EC61}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{110DF492-6624-42D0-964E-5359D5E2DB97}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -757,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B9AFA2-1031-4393-A4C4-7CF1674C8571}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,4 +1023,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88512BE-3EEE-4DD1-8DFB-D4A02567583E}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove config editor uipath form and reorganize
</commit_message>
<xml_diff>
--- a/Plugins.xlsx
+++ b/Plugins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Skiuileuf\Documents\UiPath\ActualizarePluginuriServerMinecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6A1C6C-7F5A-4C2A-BB08-BD9492CE6C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8389B7C6-7F29-4BFC-8C39-EE544EE18028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
@@ -562,7 +562,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
@@ -576,7 +576,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C5" t="s">
@@ -612,7 +612,7 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C8" t="s">
@@ -623,7 +623,7 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C9" t="s">
@@ -634,7 +634,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
@@ -648,7 +648,7 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C11" t="s">
@@ -659,7 +659,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C12" t="s">
@@ -670,7 +670,7 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C13" t="s">
@@ -681,7 +681,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C14" t="s">
@@ -692,7 +692,7 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C15" t="s">
@@ -717,7 +717,7 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
@@ -728,7 +728,7 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
@@ -742,7 +742,7 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C19" t="s">
@@ -753,7 +753,7 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C20" t="s">
@@ -764,6 +764,21 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{B9B917E1-554F-4C21-8DEF-DD1DEB24EC61}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{110DF492-6624-42D0-964E-5359D5E2DB97}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{EB5369F4-8853-4B0E-9716-D668DB8CEFFA}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{F6220F49-3746-4B98-9A5C-4B2DD878C7D2}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{5C581AB0-B354-4065-A1C5-D0196A14EFD6}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{75B5C638-2DB4-45AA-91B3-EA45620FAFA3}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{F7AC725C-A172-4775-ABF2-5F64992587E2}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{C1F5B0B9-F4A3-4345-88A9-490590817B0D}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{22AF3927-4582-4D3A-9D14-45705E96BA39}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{3136E40A-C530-45C9-9008-E45AAE7BBD04}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{8A890EA1-4BAE-4416-8B6A-7D98769A037C}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{980427A4-F104-43B9-A681-7CE8E0585F26}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{7D0961D8-B28E-4AC0-9B9C-75B16B78663F}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{DFB8C0A0-8997-4C5B-9883-D79C431BAEB1}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{A43A2FC0-58CB-4DB2-88ED-F76385388893}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{C75981EB-E896-46E1-885E-503EF4210E30}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{93A6E48B-D135-4D55-8F65-1D75B9CE2935}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>